<commit_message>
adding dash and mediator
</commit_message>
<xml_diff>
--- a/raw_data/all_data.xlsx
+++ b/raw_data/all_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lance.noel\Desktop\important\fruit_anlaysis\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A58A83-F94D-4C34-AC96-AB755B977574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550F90CE-8D99-4F19-B806-097AA874FE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-10770" windowWidth="38620" windowHeight="21220" xr2:uid="{925F1497-18F4-4D72-9FB7-5853596A5A47}"/>
   </bookViews>
@@ -581,7 +581,7 @@
   <dimension ref="A1:U44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z37" sqref="Z37"/>
+      <selection activeCell="X28" sqref="X28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
adding Dillman, Amy and Meridith
</commit_message>
<xml_diff>
--- a/raw_data/all_data.xlsx
+++ b/raw_data/all_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lance.noel\Desktop\important\fruit_anlaysis\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F4C171-E34D-46BC-BFED-B98B3A59DA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34CF1744-94F7-47A8-BEDC-58078991F4D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-10770" windowWidth="38620" windowHeight="21220" xr2:uid="{925F1497-18F4-4D72-9FB7-5853596A5A47}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>Kier</t>
   </si>
@@ -248,6 +248,15 @@
   </si>
   <si>
     <t>Talia</t>
+  </si>
+  <si>
+    <t>Meridith</t>
+  </si>
+  <si>
+    <t>Amy</t>
+  </si>
+  <si>
+    <t>Dillman</t>
   </si>
 </sst>
 </file>
@@ -599,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{324CB061-CAAA-4A80-8843-E7A82ECBBAC5}">
-  <dimension ref="A1:AB44"/>
+  <dimension ref="A1:AE44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB43" sqref="AB43"/>
+      <selection activeCell="AE45" sqref="AE45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -610,7 +619,7 @@
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -695,8 +704,17 @@
       <c r="AB1" t="s">
         <v>70</v>
       </c>
+      <c r="AC1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -781,8 +799,17 @@
       <c r="AB2">
         <v>3</v>
       </c>
+      <c r="AC2">
+        <v>4</v>
+      </c>
+      <c r="AD2">
+        <v>5</v>
+      </c>
+      <c r="AE2">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -867,8 +894,17 @@
       <c r="AB3">
         <v>5</v>
       </c>
+      <c r="AC3">
+        <v>4</v>
+      </c>
+      <c r="AD3">
+        <v>4</v>
+      </c>
+      <c r="AE3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -953,8 +989,17 @@
       <c r="AB4">
         <v>5</v>
       </c>
+      <c r="AC4">
+        <v>5</v>
+      </c>
+      <c r="AD4">
+        <v>5</v>
+      </c>
+      <c r="AE4">
+        <v>5</v>
+      </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1039,8 +1084,17 @@
       <c r="AB5">
         <v>4</v>
       </c>
+      <c r="AC5">
+        <v>3</v>
+      </c>
+      <c r="AD5">
+        <v>5</v>
+      </c>
+      <c r="AE5">
+        <v>4</v>
+      </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1125,8 +1179,17 @@
       <c r="AB6">
         <v>3</v>
       </c>
+      <c r="AC6">
+        <v>2</v>
+      </c>
+      <c r="AD6">
+        <v>4</v>
+      </c>
+      <c r="AE6">
+        <v>4</v>
+      </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1211,8 +1274,17 @@
       <c r="AB7">
         <v>5</v>
       </c>
+      <c r="AC7">
+        <v>4</v>
+      </c>
+      <c r="AD7">
+        <v>5</v>
+      </c>
+      <c r="AE7">
+        <v>5</v>
+      </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1297,8 +1369,17 @@
       <c r="AB8">
         <v>2</v>
       </c>
+      <c r="AC8">
+        <v>3</v>
+      </c>
+      <c r="AD8">
+        <v>1</v>
+      </c>
+      <c r="AE8">
+        <v>3</v>
+      </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1383,8 +1464,17 @@
       <c r="AB9">
         <v>3</v>
       </c>
+      <c r="AC9">
+        <v>3</v>
+      </c>
+      <c r="AD9">
+        <v>5</v>
+      </c>
+      <c r="AE9">
+        <v>3</v>
+      </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1469,8 +1559,17 @@
       <c r="AB10">
         <v>1</v>
       </c>
+      <c r="AC10">
+        <v>3</v>
+      </c>
+      <c r="AD10">
+        <v>4</v>
+      </c>
+      <c r="AE10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1555,8 +1654,17 @@
       <c r="AB11">
         <v>4</v>
       </c>
+      <c r="AC11">
+        <v>5</v>
+      </c>
+      <c r="AD11">
+        <v>4</v>
+      </c>
+      <c r="AE11">
+        <v>4</v>
+      </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1641,8 +1749,17 @@
       <c r="AB12">
         <v>2</v>
       </c>
+      <c r="AC12">
+        <v>2</v>
+      </c>
+      <c r="AD12">
+        <v>3</v>
+      </c>
+      <c r="AE12">
+        <v>3</v>
+      </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1727,8 +1844,17 @@
       <c r="AB13">
         <v>5</v>
       </c>
+      <c r="AC13">
+        <v>3</v>
+      </c>
+      <c r="AD13">
+        <v>3</v>
+      </c>
+      <c r="AE13">
+        <v>4</v>
+      </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1813,8 +1939,17 @@
       <c r="AB14">
         <v>4</v>
       </c>
+      <c r="AC14">
+        <v>1</v>
+      </c>
+      <c r="AD14">
+        <v>5</v>
+      </c>
+      <c r="AE14">
+        <v>4</v>
+      </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1899,8 +2034,17 @@
       <c r="AB15">
         <v>5</v>
       </c>
+      <c r="AC15">
+        <v>5</v>
+      </c>
+      <c r="AD15">
+        <v>5</v>
+      </c>
+      <c r="AE15">
+        <v>4</v>
+      </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1985,8 +2129,17 @@
       <c r="AB16">
         <v>3</v>
       </c>
+      <c r="AC16">
+        <v>5</v>
+      </c>
+      <c r="AD16">
+        <v>5</v>
+      </c>
+      <c r="AE16">
+        <v>5</v>
+      </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -2071,8 +2224,17 @@
       <c r="AB17">
         <v>4</v>
       </c>
+      <c r="AC17">
+        <v>5</v>
+      </c>
+      <c r="AD17">
+        <v>4</v>
+      </c>
+      <c r="AE17">
+        <v>2</v>
+      </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -2157,8 +2319,17 @@
       <c r="AB18">
         <v>3</v>
       </c>
+      <c r="AC18">
+        <v>5</v>
+      </c>
+      <c r="AD18">
+        <v>4</v>
+      </c>
+      <c r="AE18">
+        <v>2</v>
+      </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -2243,8 +2414,17 @@
       <c r="AB19">
         <v>2</v>
       </c>
+      <c r="AC19">
+        <v>2</v>
+      </c>
+      <c r="AD19">
+        <v>1</v>
+      </c>
+      <c r="AE19">
+        <v>4</v>
+      </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2329,8 +2509,17 @@
       <c r="AB20">
         <v>5</v>
       </c>
+      <c r="AC20">
+        <v>1</v>
+      </c>
+      <c r="AD20">
+        <v>1</v>
+      </c>
+      <c r="AE20">
+        <v>2</v>
+      </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -2415,8 +2604,17 @@
       <c r="AB21">
         <v>5</v>
       </c>
+      <c r="AC21">
+        <v>4</v>
+      </c>
+      <c r="AD21">
+        <v>4</v>
+      </c>
+      <c r="AE21">
+        <v>4</v>
+      </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -2501,8 +2699,17 @@
       <c r="AB22">
         <v>2</v>
       </c>
+      <c r="AC22">
+        <v>2</v>
+      </c>
+      <c r="AD22">
+        <v>2</v>
+      </c>
+      <c r="AE22">
+        <v>4</v>
+      </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -2587,8 +2794,17 @@
       <c r="AB23">
         <v>5</v>
       </c>
+      <c r="AC23">
+        <v>4</v>
+      </c>
+      <c r="AD23">
+        <v>3</v>
+      </c>
+      <c r="AE23">
+        <v>4</v>
+      </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -2673,8 +2889,17 @@
       <c r="AB24">
         <v>2</v>
       </c>
+      <c r="AC24">
+        <v>3</v>
+      </c>
+      <c r="AD24">
+        <v>2</v>
+      </c>
+      <c r="AE24">
+        <v>3</v>
+      </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -2759,8 +2984,17 @@
       <c r="AB25">
         <v>3</v>
       </c>
+      <c r="AC25">
+        <v>5</v>
+      </c>
+      <c r="AD25">
+        <v>5</v>
+      </c>
+      <c r="AE25">
+        <v>3</v>
+      </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -2845,8 +3079,17 @@
       <c r="AB26">
         <v>5</v>
       </c>
+      <c r="AC26">
+        <v>4</v>
+      </c>
+      <c r="AD26">
+        <v>2</v>
+      </c>
+      <c r="AE26">
+        <v>4</v>
+      </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2931,8 +3174,17 @@
       <c r="AB27">
         <v>4</v>
       </c>
+      <c r="AC27">
+        <v>4</v>
+      </c>
+      <c r="AD27">
+        <v>3</v>
+      </c>
+      <c r="AE27">
+        <v>3</v>
+      </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -3017,8 +3269,17 @@
       <c r="AB28">
         <v>4</v>
       </c>
+      <c r="AC28">
+        <v>4</v>
+      </c>
+      <c r="AD28">
+        <v>3</v>
+      </c>
+      <c r="AE28">
+        <v>2</v>
+      </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -3103,8 +3364,17 @@
       <c r="AB29">
         <v>1</v>
       </c>
+      <c r="AC29">
+        <v>1</v>
+      </c>
+      <c r="AD29">
+        <v>2</v>
+      </c>
+      <c r="AE29">
+        <v>4</v>
+      </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -3189,8 +3459,17 @@
       <c r="AB30">
         <v>4</v>
       </c>
+      <c r="AC30">
+        <v>1</v>
+      </c>
+      <c r="AD30">
+        <v>3</v>
+      </c>
+      <c r="AE30">
+        <v>4</v>
+      </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -3275,8 +3554,17 @@
       <c r="AB31">
         <v>2</v>
       </c>
+      <c r="AC31">
+        <v>3</v>
+      </c>
+      <c r="AD31">
+        <v>2</v>
+      </c>
+      <c r="AE31">
+        <v>2</v>
+      </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -3361,8 +3649,17 @@
       <c r="AB32">
         <v>3</v>
       </c>
+      <c r="AC32">
+        <v>3</v>
+      </c>
+      <c r="AD32">
+        <v>2</v>
+      </c>
+      <c r="AE32">
+        <v>3</v>
+      </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -3447,8 +3744,17 @@
       <c r="AB33">
         <v>5</v>
       </c>
+      <c r="AC33">
+        <v>4</v>
+      </c>
+      <c r="AD33">
+        <v>3</v>
+      </c>
+      <c r="AE33">
+        <v>3</v>
+      </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -3533,8 +3839,17 @@
       <c r="AB34">
         <v>3</v>
       </c>
+      <c r="AC34">
+        <v>4</v>
+      </c>
+      <c r="AD34">
+        <v>3</v>
+      </c>
+      <c r="AE34">
+        <v>3</v>
+      </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -3619,8 +3934,17 @@
       <c r="AB35">
         <v>4</v>
       </c>
+      <c r="AC35">
+        <v>1</v>
+      </c>
+      <c r="AD35">
+        <v>4</v>
+      </c>
+      <c r="AE35">
+        <v>2</v>
+      </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -3705,8 +4029,17 @@
       <c r="AB36">
         <v>3</v>
       </c>
+      <c r="AC36">
+        <v>2</v>
+      </c>
+      <c r="AD36">
+        <v>2</v>
+      </c>
+      <c r="AE36">
+        <v>3</v>
+      </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -3791,8 +4124,17 @@
       <c r="AB37">
         <v>1</v>
       </c>
+      <c r="AC37">
+        <v>3</v>
+      </c>
+      <c r="AD37">
+        <v>4</v>
+      </c>
+      <c r="AE37">
+        <v>5</v>
+      </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>33</v>
       </c>
@@ -3877,8 +4219,17 @@
       <c r="AB38">
         <v>2</v>
       </c>
+      <c r="AC38">
+        <v>2</v>
+      </c>
+      <c r="AD38">
+        <v>1</v>
+      </c>
+      <c r="AE38">
+        <v>3</v>
+      </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>51</v>
       </c>
@@ -3963,8 +4314,17 @@
       <c r="AB39">
         <v>4</v>
       </c>
+      <c r="AC39">
+        <v>2</v>
+      </c>
+      <c r="AD39">
+        <v>5</v>
+      </c>
+      <c r="AE39">
+        <v>4</v>
+      </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -4049,8 +4409,17 @@
       <c r="AB40">
         <v>1</v>
       </c>
+      <c r="AC40">
+        <v>4</v>
+      </c>
+      <c r="AD40">
+        <v>2</v>
+      </c>
+      <c r="AE40">
+        <v>3</v>
+      </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>34</v>
       </c>
@@ -4135,8 +4504,17 @@
       <c r="AB41">
         <v>1</v>
       </c>
+      <c r="AC41">
+        <v>2</v>
+      </c>
+      <c r="AD41">
+        <v>1</v>
+      </c>
+      <c r="AE41">
+        <v>1</v>
+      </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>37</v>
       </c>
@@ -4221,8 +4599,17 @@
       <c r="AB42">
         <v>-99</v>
       </c>
+      <c r="AC42">
+        <v>2</v>
+      </c>
+      <c r="AD42">
+        <v>1</v>
+      </c>
+      <c r="AE42">
+        <v>2</v>
+      </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>39</v>
       </c>
@@ -4307,8 +4694,17 @@
       <c r="AB43">
         <v>3</v>
       </c>
+      <c r="AC43">
+        <v>1</v>
+      </c>
+      <c r="AD43">
+        <v>1</v>
+      </c>
+      <c r="AE43">
+        <v>1</v>
+      </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -4392,6 +4788,15 @@
       </c>
       <c r="AB44">
         <v>2</v>
+      </c>
+      <c r="AC44">
+        <v>1</v>
+      </c>
+      <c r="AD44">
+        <v>3</v>
+      </c>
+      <c r="AE44">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>